<commit_message>
Add consent form and lists of prompts for participants
</commit_message>
<xml_diff>
--- a/pilot/pilotA.xlsx
+++ b/pilot/pilotA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shivani Guptasarma\Documents\santello1998\pilot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D8A6A4F-B753-4CE3-A195-05272E72241A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E9F23CD-66B4-48F2-8C60-129A47069462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{F2D30B77-542E-4B52-9A82-C37032AB9989}"/>
+    <workbookView xWindow="-1488" yWindow="2160" windowWidth="17280" windowHeight="8964" tabRatio="895" xr2:uid="{F2D30B77-542E-4B52-9A82-C37032AB9989}"/>
   </bookViews>
   <sheets>
     <sheet name="ListGeneration" sheetId="1" r:id="rId1"/>
@@ -655,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26249B82-5ACF-4283-881E-123F1D663BD5}">
   <dimension ref="A1:S171"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1:S1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -670,7 +670,7 @@
       </c>
       <c r="B1">
         <f t="shared" ref="B1:B32" ca="1" si="0">RAND()</f>
-        <v>0.66737373104272912</v>
+        <v>0.23904324015396716</v>
       </c>
       <c r="M1" t="s">
         <v>0</v>
@@ -700,7 +700,7 @@
       </c>
       <c r="B2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.5071738913116578</v>
+        <v>0.49775531523131844</v>
       </c>
       <c r="M2" t="s">
         <v>1</v>
@@ -730,7 +730,7 @@
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.20344068215494082</v>
+        <v>0.27007583474839503</v>
       </c>
       <c r="M3" t="s">
         <v>2</v>
@@ -760,7 +760,7 @@
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.21366992354675163</v>
+        <v>0.79156621549245298</v>
       </c>
       <c r="M4" t="s">
         <v>3</v>
@@ -790,7 +790,7 @@
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>8.8246788853111657E-2</v>
+        <v>0.37186105052999496</v>
       </c>
       <c r="M5" t="s">
         <v>4</v>
@@ -820,7 +820,7 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.63424060534263227</v>
+        <v>0.40139129462581757</v>
       </c>
       <c r="M6" t="s">
         <v>5</v>
@@ -850,7 +850,7 @@
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.33320399218955266</v>
+        <v>0.66444554990373572</v>
       </c>
       <c r="M7" t="s">
         <v>6</v>
@@ -880,7 +880,7 @@
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.46816674254786483</v>
+        <v>6.9059088173116789E-2</v>
       </c>
       <c r="M8" t="s">
         <v>7</v>
@@ -910,7 +910,7 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>0.66260233421034664</v>
+        <v>0.33614147288151175</v>
       </c>
       <c r="M9" t="s">
         <v>8</v>
@@ -940,7 +940,7 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>0.15885958461862071</v>
+        <v>0.69645932430083868</v>
       </c>
       <c r="M10" t="s">
         <v>9</v>
@@ -970,7 +970,7 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.33965734567472061</v>
+        <v>0.26095354932578585</v>
       </c>
       <c r="M11" t="s">
         <v>10</v>
@@ -1000,7 +1000,7 @@
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.75986048251052118</v>
+        <v>0.58758190786008035</v>
       </c>
       <c r="M12" t="s">
         <v>11</v>
@@ -1030,7 +1030,7 @@
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.15273842807959603</v>
+        <v>0.38387582803353371</v>
       </c>
       <c r="M13" t="s">
         <v>12</v>
@@ -1060,7 +1060,7 @@
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>0.83782962760509394</v>
+        <v>0.70723126690095584</v>
       </c>
       <c r="M14" t="s">
         <v>13</v>
@@ -1090,7 +1090,7 @@
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>0.28994501121253669</v>
+        <v>0.59044632235457883</v>
       </c>
       <c r="M15" t="s">
         <v>14</v>
@@ -1120,7 +1120,7 @@
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.83851544965287728</v>
+        <v>0.77458445108712504</v>
       </c>
       <c r="M16" t="s">
         <v>15</v>
@@ -1150,7 +1150,7 @@
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="0"/>
-        <v>8.6596808747253506E-3</v>
+        <v>0.9189563536309977</v>
       </c>
       <c r="M17" t="s">
         <v>16</v>
@@ -1180,7 +1180,7 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="0"/>
-        <v>0.47782914868987891</v>
+        <v>0.9173624972039861</v>
       </c>
       <c r="M18" t="s">
         <v>17</v>
@@ -1210,7 +1210,7 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="0"/>
-        <v>0.37172755455918971</v>
+        <v>0.6473226691391647</v>
       </c>
       <c r="M19" t="s">
         <v>18</v>
@@ -1240,7 +1240,7 @@
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="0"/>
-        <v>0.71166720358379665</v>
+        <v>0.31893047511796502</v>
       </c>
       <c r="M20" t="s">
         <v>19</v>
@@ -1270,7 +1270,7 @@
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="0"/>
-        <v>0.29559893828115913</v>
+        <v>0.21458688815515881</v>
       </c>
       <c r="M21" t="s">
         <v>20</v>
@@ -1300,7 +1300,7 @@
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="0"/>
-        <v>0.6286926747690943</v>
+        <v>0.7782090959450485</v>
       </c>
       <c r="M22" t="s">
         <v>21</v>
@@ -1330,7 +1330,7 @@
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="0"/>
-        <v>5.6676972513336588E-2</v>
+        <v>0.35562460343463653</v>
       </c>
       <c r="M23" t="s">
         <v>22</v>
@@ -1360,7 +1360,7 @@
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="0"/>
-        <v>0.16372743858194416</v>
+        <v>0.50357113906926654</v>
       </c>
       <c r="M24" t="s">
         <v>23</v>
@@ -1390,7 +1390,7 @@
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="0"/>
-        <v>0.20943198217804615</v>
+        <v>0.62783987511399475</v>
       </c>
       <c r="M25" t="s">
         <v>24</v>
@@ -1420,7 +1420,7 @@
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="0"/>
-        <v>0.60108557603201218</v>
+        <v>0.8277226765943555</v>
       </c>
       <c r="M26" t="s">
         <v>25</v>
@@ -1450,7 +1450,7 @@
       </c>
       <c r="B27">
         <f t="shared" ca="1" si="0"/>
-        <v>0.78183901732835426</v>
+        <v>0.84886370555555335</v>
       </c>
       <c r="M27" t="s">
         <v>26</v>
@@ -1480,7 +1480,7 @@
       </c>
       <c r="B28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.19764834602623149</v>
+        <v>0.60705671455160104</v>
       </c>
       <c r="M28" t="s">
         <v>27</v>
@@ -1510,7 +1510,7 @@
       </c>
       <c r="B29">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2097244900630577E-2</v>
+        <v>0.25811561663763594</v>
       </c>
       <c r="M29" t="s">
         <v>28</v>
@@ -1540,7 +1540,7 @@
       </c>
       <c r="B30">
         <f t="shared" ca="1" si="0"/>
-        <v>0.45301447388671445</v>
+        <v>0.39177293760675569</v>
       </c>
       <c r="M30" t="s">
         <v>29</v>
@@ -1570,7 +1570,7 @@
       </c>
       <c r="B31">
         <f t="shared" ca="1" si="0"/>
-        <v>0.76187090462775287</v>
+        <v>0.62909904054578414</v>
       </c>
       <c r="M31" t="s">
         <v>30</v>
@@ -1600,7 +1600,7 @@
       </c>
       <c r="B32">
         <f t="shared" ca="1" si="0"/>
-        <v>0.68845552638522378</v>
+        <v>0.17408655109951332</v>
       </c>
       <c r="M32" t="s">
         <v>31</v>
@@ -1630,7 +1630,7 @@
       </c>
       <c r="B33">
         <f t="shared" ref="B33:B64" ca="1" si="1">RAND()</f>
-        <v>0.64405681575952134</v>
+        <v>9.0535962240783863E-2</v>
       </c>
       <c r="M33" t="s">
         <v>32</v>
@@ -1660,7 +1660,7 @@
       </c>
       <c r="B34">
         <f t="shared" ca="1" si="1"/>
-        <v>0.22667211625112227</v>
+        <v>0.92055395264129436</v>
       </c>
       <c r="M34" t="s">
         <v>33</v>
@@ -1690,7 +1690,7 @@
       </c>
       <c r="B35">
         <f t="shared" ca="1" si="1"/>
-        <v>4.3977378364485897E-2</v>
+        <v>0.97762643756199363</v>
       </c>
       <c r="M35" t="s">
         <v>34</v>
@@ -1720,7 +1720,7 @@
       </c>
       <c r="B36">
         <f t="shared" ca="1" si="1"/>
-        <v>0.25078568575720128</v>
+        <v>0.25926047425465926</v>
       </c>
       <c r="M36" t="s">
         <v>35</v>
@@ -1750,7 +1750,7 @@
       </c>
       <c r="B37">
         <f t="shared" ca="1" si="1"/>
-        <v>0.70347479757567244</v>
+        <v>0.47866788032678775</v>
       </c>
       <c r="M37" t="s">
         <v>36</v>
@@ -1780,7 +1780,7 @@
       </c>
       <c r="B38">
         <f t="shared" ca="1" si="1"/>
-        <v>0.70507653580072427</v>
+        <v>3.4234600134470439E-2</v>
       </c>
       <c r="M38" t="s">
         <v>37</v>
@@ -1810,7 +1810,7 @@
       </c>
       <c r="B39">
         <f t="shared" ca="1" si="1"/>
-        <v>0.92592579035169542</v>
+        <v>0.78689725209035866</v>
       </c>
       <c r="M39" t="s">
         <v>38</v>
@@ -1840,7 +1840,7 @@
       </c>
       <c r="B40">
         <f t="shared" ca="1" si="1"/>
-        <v>0.15780043517734399</v>
+        <v>0.19539656620114043</v>
       </c>
       <c r="M40" t="s">
         <v>39</v>
@@ -1870,7 +1870,7 @@
       </c>
       <c r="B41">
         <f t="shared" ca="1" si="1"/>
-        <v>0.35555134017741952</v>
+        <v>0.75131575030395847</v>
       </c>
       <c r="M41" t="s">
         <v>40</v>
@@ -1900,7 +1900,7 @@
       </c>
       <c r="B42">
         <f t="shared" ca="1" si="1"/>
-        <v>0.46318146456594333</v>
+        <v>5.8933633039935929E-2</v>
       </c>
       <c r="M42" t="s">
         <v>41</v>
@@ -1930,7 +1930,7 @@
       </c>
       <c r="B43">
         <f t="shared" ca="1" si="1"/>
-        <v>0.55101239546465974</v>
+        <v>0.73342166479022453</v>
       </c>
       <c r="M43" t="s">
         <v>42</v>
@@ -1960,7 +1960,7 @@
       </c>
       <c r="B44">
         <f t="shared" ca="1" si="1"/>
-        <v>0.36899355597537131</v>
+        <v>0.98333981979669749</v>
       </c>
       <c r="M44" t="s">
         <v>43</v>
@@ -1990,7 +1990,7 @@
       </c>
       <c r="B45">
         <f t="shared" ca="1" si="1"/>
-        <v>3.2403539018476035E-2</v>
+        <v>0.78859720740032868</v>
       </c>
       <c r="M45" t="s">
         <v>44</v>
@@ -2020,7 +2020,7 @@
       </c>
       <c r="B46">
         <f t="shared" ca="1" si="1"/>
-        <v>0.33975573101492085</v>
+        <v>1.3968578874227977E-2</v>
       </c>
       <c r="M46" t="s">
         <v>45</v>
@@ -2050,7 +2050,7 @@
       </c>
       <c r="B47">
         <f t="shared" ca="1" si="1"/>
-        <v>0.27272315789448609</v>
+        <v>0.55163277892427609</v>
       </c>
       <c r="M47" t="s">
         <v>46</v>
@@ -2080,7 +2080,7 @@
       </c>
       <c r="B48">
         <f t="shared" ca="1" si="1"/>
-        <v>0.88785200746322901</v>
+        <v>0.43606009410595969</v>
       </c>
       <c r="M48" t="s">
         <v>47</v>
@@ -2110,7 +2110,7 @@
       </c>
       <c r="B49">
         <f t="shared" ca="1" si="1"/>
-        <v>5.5852523133057441E-2</v>
+        <v>0.16339983206951603</v>
       </c>
       <c r="M49" t="s">
         <v>48</v>
@@ -2140,7 +2140,7 @@
       </c>
       <c r="B50">
         <f t="shared" ca="1" si="1"/>
-        <v>0.34854620233973543</v>
+        <v>0.83870188631973419</v>
       </c>
       <c r="M50" t="s">
         <v>49</v>
@@ -2170,7 +2170,7 @@
       </c>
       <c r="B51">
         <f t="shared" ca="1" si="1"/>
-        <v>0.94687947017718999</v>
+        <v>0.53135675391667292</v>
       </c>
       <c r="M51" t="s">
         <v>50</v>
@@ -2200,7 +2200,7 @@
       </c>
       <c r="B52">
         <f t="shared" ca="1" si="1"/>
-        <v>0.12425023058156337</v>
+        <v>0.35570977965345563</v>
       </c>
       <c r="M52" t="s">
         <v>51</v>
@@ -2230,7 +2230,7 @@
       </c>
       <c r="B53">
         <f t="shared" ca="1" si="1"/>
-        <v>0.5462196810504687</v>
+        <v>0.48941241374389433</v>
       </c>
       <c r="M53" t="s">
         <v>52</v>
@@ -2260,7 +2260,7 @@
       </c>
       <c r="B54">
         <f t="shared" ca="1" si="1"/>
-        <v>0.64037413173980406</v>
+        <v>0.60763701241171197</v>
       </c>
       <c r="M54" t="s">
         <v>53</v>
@@ -2290,7 +2290,7 @@
       </c>
       <c r="B55">
         <f t="shared" ca="1" si="1"/>
-        <v>0.96424056618243847</v>
+        <v>0.59462146541227467</v>
       </c>
       <c r="M55" t="s">
         <v>54</v>
@@ -2320,7 +2320,7 @@
       </c>
       <c r="B56">
         <f t="shared" ca="1" si="1"/>
-        <v>0.66580626504385254</v>
+        <v>4.7359116698312831E-2</v>
       </c>
       <c r="M56" t="s">
         <v>55</v>
@@ -2350,7 +2350,7 @@
       </c>
       <c r="B57">
         <f t="shared" ca="1" si="1"/>
-        <v>0.32746896763423117</v>
+        <v>0.8124043029701824</v>
       </c>
       <c r="M57" t="s">
         <v>56</v>
@@ -2380,7 +2380,7 @@
       </c>
       <c r="B58">
         <f t="shared" ca="1" si="1"/>
-        <v>0.49343991754434757</v>
+        <v>2.7463556131008038E-2</v>
       </c>
       <c r="N58" t="s">
         <v>40</v>
@@ -2407,7 +2407,7 @@
       </c>
       <c r="B59">
         <f t="shared" ca="1" si="1"/>
-        <v>0.59673206376138721</v>
+        <v>0.64291832528623871</v>
       </c>
       <c r="N59" t="s">
         <v>29</v>
@@ -2434,7 +2434,7 @@
       </c>
       <c r="B60">
         <f t="shared" ca="1" si="1"/>
-        <v>0.86471211564950368</v>
+        <v>0.47724470274482045</v>
       </c>
       <c r="N60" t="s">
         <v>16</v>
@@ -2461,7 +2461,7 @@
       </c>
       <c r="B61">
         <f t="shared" ca="1" si="1"/>
-        <v>0.63789742504515745</v>
+        <v>0.50668637506691339</v>
       </c>
       <c r="N61" t="s">
         <v>53</v>
@@ -2488,7 +2488,7 @@
       </c>
       <c r="B62">
         <f t="shared" ca="1" si="1"/>
-        <v>0.12899285316981535</v>
+        <v>0.2280413532356913</v>
       </c>
       <c r="N62" t="s">
         <v>49</v>
@@ -2515,7 +2515,7 @@
       </c>
       <c r="B63">
         <f t="shared" ca="1" si="1"/>
-        <v>0.55784068976816081</v>
+        <v>0.80774770552395125</v>
       </c>
       <c r="N63" t="s">
         <v>6</v>
@@ -2542,7 +2542,7 @@
       </c>
       <c r="B64">
         <f t="shared" ca="1" si="1"/>
-        <v>0.71491964855183188</v>
+        <v>0.85758306892676517</v>
       </c>
       <c r="N64" t="s">
         <v>31</v>
@@ -2569,7 +2569,7 @@
       </c>
       <c r="B65">
         <f t="shared" ref="B65:B96" ca="1" si="2">RAND()</f>
-        <v>0.69851948965553723</v>
+        <v>0.95074820265621829</v>
       </c>
       <c r="N65" t="s">
         <v>55</v>
@@ -2596,7 +2596,7 @@
       </c>
       <c r="B66">
         <f t="shared" ca="1" si="2"/>
-        <v>0.2698518716400321</v>
+        <v>0.51025504264511468</v>
       </c>
       <c r="N66" t="s">
         <v>8</v>
@@ -2623,7 +2623,7 @@
       </c>
       <c r="B67">
         <f t="shared" ca="1" si="2"/>
-        <v>0.73388519197631308</v>
+        <v>0.10095700312040112</v>
       </c>
       <c r="N67" t="s">
         <v>25</v>
@@ -2650,7 +2650,7 @@
       </c>
       <c r="B68">
         <f t="shared" ca="1" si="2"/>
-        <v>0.84632974758869628</v>
+        <v>0.5032929724594587</v>
       </c>
       <c r="N68" t="s">
         <v>31</v>
@@ -2677,7 +2677,7 @@
       </c>
       <c r="B69">
         <f t="shared" ca="1" si="2"/>
-        <v>0.56364490782022392</v>
+        <v>0.70102458462337169</v>
       </c>
       <c r="N69" t="s">
         <v>19</v>
@@ -2704,7 +2704,7 @@
       </c>
       <c r="B70">
         <f t="shared" ca="1" si="2"/>
-        <v>0.47450176309860326</v>
+        <v>0.96627131257819121</v>
       </c>
       <c r="N70" t="s">
         <v>39</v>
@@ -2731,7 +2731,7 @@
       </c>
       <c r="B71">
         <f t="shared" ca="1" si="2"/>
-        <v>0.27126752406487642</v>
+        <v>0.972217329130456</v>
       </c>
       <c r="N71" t="s">
         <v>52</v>
@@ -2758,7 +2758,7 @@
       </c>
       <c r="B72">
         <f t="shared" ca="1" si="2"/>
-        <v>0.75148399003634281</v>
+        <v>0.44040267948809253</v>
       </c>
       <c r="N72" t="s">
         <v>28</v>
@@ -2785,7 +2785,7 @@
       </c>
       <c r="B73">
         <f t="shared" ca="1" si="2"/>
-        <v>0.30140562954999661</v>
+        <v>0.28805008233985296</v>
       </c>
       <c r="N73" t="s">
         <v>22</v>
@@ -2812,7 +2812,7 @@
       </c>
       <c r="B74">
         <f t="shared" ca="1" si="2"/>
-        <v>0.16391745599730245</v>
+        <v>0.68950395169890055</v>
       </c>
       <c r="N74" t="s">
         <v>56</v>
@@ -2839,7 +2839,7 @@
       </c>
       <c r="B75">
         <f t="shared" ca="1" si="2"/>
-        <v>0.40764728750790369</v>
+        <v>0.15354331801169718</v>
       </c>
       <c r="N75" t="s">
         <v>47</v>
@@ -2866,7 +2866,7 @@
       </c>
       <c r="B76">
         <f t="shared" ca="1" si="2"/>
-        <v>0.31339691407619519</v>
+        <v>0.56920731606987807</v>
       </c>
       <c r="N76" t="s">
         <v>26</v>
@@ -2893,7 +2893,7 @@
       </c>
       <c r="B77">
         <f t="shared" ca="1" si="2"/>
-        <v>0.22995124026389535</v>
+        <v>0.96611923511881848</v>
       </c>
       <c r="N77" t="s">
         <v>20</v>
@@ -2920,7 +2920,7 @@
       </c>
       <c r="B78">
         <f t="shared" ca="1" si="2"/>
-        <v>0.47572503799950627</v>
+        <v>0.64579792026915317</v>
       </c>
       <c r="N78" t="s">
         <v>9</v>
@@ -2947,7 +2947,7 @@
       </c>
       <c r="B79">
         <f t="shared" ca="1" si="2"/>
-        <v>0.43750465982356324</v>
+        <v>0.51871334291983939</v>
       </c>
       <c r="N79" t="s">
         <v>41</v>
@@ -2974,7 +2974,7 @@
       </c>
       <c r="B80">
         <f t="shared" ca="1" si="2"/>
-        <v>0.84867230842521491</v>
+        <v>0.42185493240187433</v>
       </c>
       <c r="N80" t="s">
         <v>12</v>
@@ -3001,7 +3001,7 @@
       </c>
       <c r="B81">
         <f t="shared" ca="1" si="2"/>
-        <v>0.90726435659565896</v>
+        <v>0.37443898001041309</v>
       </c>
       <c r="N81" t="s">
         <v>27</v>
@@ -3028,7 +3028,7 @@
       </c>
       <c r="B82">
         <f t="shared" ca="1" si="2"/>
-        <v>5.9359388390668455E-2</v>
+        <v>8.3272329490952091E-3</v>
       </c>
       <c r="N82" t="s">
         <v>32</v>
@@ -3055,7 +3055,7 @@
       </c>
       <c r="B83">
         <f t="shared" ca="1" si="2"/>
-        <v>0.78925370321389843</v>
+        <v>0.94153495332335124</v>
       </c>
       <c r="N83" t="s">
         <v>33</v>
@@ -3082,7 +3082,7 @@
       </c>
       <c r="B84">
         <f t="shared" ca="1" si="2"/>
-        <v>0.88027509018949734</v>
+        <v>0.62161340764774764</v>
       </c>
       <c r="N84" t="s">
         <v>50</v>
@@ -3109,7 +3109,7 @@
       </c>
       <c r="B85">
         <f t="shared" ca="1" si="2"/>
-        <v>0.35134403300557038</v>
+        <v>0.4056830576006325</v>
       </c>
       <c r="N85" t="s">
         <v>4</v>
@@ -3136,7 +3136,7 @@
       </c>
       <c r="B86">
         <f t="shared" ca="1" si="2"/>
-        <v>0.39174284749562394</v>
+        <v>0.13851336877410469</v>
       </c>
       <c r="N86" t="s">
         <v>37</v>
@@ -3163,7 +3163,7 @@
       </c>
       <c r="B87">
         <f t="shared" ca="1" si="2"/>
-        <v>0.67154499864547645</v>
+        <v>0.47540112834608328</v>
       </c>
       <c r="N87" t="s">
         <v>47</v>
@@ -3190,7 +3190,7 @@
       </c>
       <c r="B88">
         <f t="shared" ca="1" si="2"/>
-        <v>0.97163450308218802</v>
+        <v>0.12160807004135132</v>
       </c>
       <c r="N88" t="s">
         <v>4</v>
@@ -3217,7 +3217,7 @@
       </c>
       <c r="B89">
         <f t="shared" ca="1" si="2"/>
-        <v>0.93022077416728599</v>
+        <v>8.3832454524588096E-2</v>
       </c>
       <c r="N89" t="s">
         <v>40</v>
@@ -3244,7 +3244,7 @@
       </c>
       <c r="B90">
         <f t="shared" ca="1" si="2"/>
-        <v>0.80055036127215706</v>
+        <v>0.6017085455673582</v>
       </c>
       <c r="N90" t="s">
         <v>13</v>
@@ -3271,7 +3271,7 @@
       </c>
       <c r="B91">
         <f t="shared" ca="1" si="2"/>
-        <v>0.21350617469173838</v>
+        <v>0.71025793231794132</v>
       </c>
       <c r="N91" t="s">
         <v>38</v>
@@ -3298,7 +3298,7 @@
       </c>
       <c r="B92">
         <f t="shared" ca="1" si="2"/>
-        <v>0.81062288948214922</v>
+        <v>0.36938093812980011</v>
       </c>
       <c r="N92" t="s">
         <v>29</v>
@@ -3325,7 +3325,7 @@
       </c>
       <c r="B93">
         <f t="shared" ca="1" si="2"/>
-        <v>0.76506355620738498</v>
+        <v>0.5496167961474141</v>
       </c>
       <c r="N93" t="s">
         <v>4</v>
@@ -3352,7 +3352,7 @@
       </c>
       <c r="B94">
         <f t="shared" ca="1" si="2"/>
-        <v>0.2857513850300436</v>
+        <v>0.87598535366088104</v>
       </c>
       <c r="N94" t="s">
         <v>6</v>
@@ -3379,7 +3379,7 @@
       </c>
       <c r="B95">
         <f t="shared" ca="1" si="2"/>
-        <v>0.85322267538418739</v>
+        <v>0.33252796829174291</v>
       </c>
       <c r="N95" t="s">
         <v>51</v>
@@ -3406,7 +3406,7 @@
       </c>
       <c r="B96">
         <f t="shared" ca="1" si="2"/>
-        <v>0.85326474525643481</v>
+        <v>0.71133818730004095</v>
       </c>
       <c r="N96" t="s">
         <v>24</v>
@@ -3433,7 +3433,7 @@
       </c>
       <c r="B97">
         <f t="shared" ref="B97:B128" ca="1" si="3">RAND()</f>
-        <v>9.741035400216902E-2</v>
+        <v>0.59567987305354875</v>
       </c>
       <c r="N97" t="s">
         <v>27</v>
@@ -3460,7 +3460,7 @@
       </c>
       <c r="B98">
         <f t="shared" ca="1" si="3"/>
-        <v>0.85724421626307934</v>
+        <v>0.93195490624010502</v>
       </c>
       <c r="N98" t="s">
         <v>41</v>
@@ -3487,7 +3487,7 @@
       </c>
       <c r="B99">
         <f t="shared" ca="1" si="3"/>
-        <v>0.91185576561042059</v>
+        <v>0.56041083461276697</v>
       </c>
       <c r="N99" t="s">
         <v>49</v>
@@ -3514,7 +3514,7 @@
       </c>
       <c r="B100">
         <f t="shared" ca="1" si="3"/>
-        <v>0.38659665722987457</v>
+        <v>0.92859070969650848</v>
       </c>
       <c r="N100" t="s">
         <v>20</v>
@@ -3541,7 +3541,7 @@
       </c>
       <c r="B101">
         <f t="shared" ca="1" si="3"/>
-        <v>0.63778417551448141</v>
+        <v>0.2822214646334581</v>
       </c>
       <c r="N101" t="s">
         <v>17</v>
@@ -3568,7 +3568,7 @@
       </c>
       <c r="B102">
         <f t="shared" ca="1" si="3"/>
-        <v>8.5019421894681368E-2</v>
+        <v>0.60218146169388531</v>
       </c>
       <c r="N102" t="s">
         <v>43</v>
@@ -3595,7 +3595,7 @@
       </c>
       <c r="B103">
         <f t="shared" ca="1" si="3"/>
-        <v>0.48803140254511901</v>
+        <v>9.765670707487506E-2</v>
       </c>
       <c r="N103" t="s">
         <v>33</v>
@@ -3622,7 +3622,7 @@
       </c>
       <c r="B104">
         <f t="shared" ca="1" si="3"/>
-        <v>0.28399063192468699</v>
+        <v>0.59668766339499846</v>
       </c>
       <c r="N104" t="s">
         <v>46</v>
@@ -3649,7 +3649,7 @@
       </c>
       <c r="B105">
         <f t="shared" ca="1" si="3"/>
-        <v>0.82888762518281422</v>
+        <v>0.96473111627268704</v>
       </c>
       <c r="N105" t="s">
         <v>24</v>
@@ -3676,7 +3676,7 @@
       </c>
       <c r="B106">
         <f t="shared" ca="1" si="3"/>
-        <v>0.36374673036413219</v>
+        <v>0.68680357274503279</v>
       </c>
       <c r="N106" t="s">
         <v>1</v>
@@ -3703,7 +3703,7 @@
       </c>
       <c r="B107">
         <f t="shared" ca="1" si="3"/>
-        <v>0.15584654049439395</v>
+        <v>0.61597097719627691</v>
       </c>
       <c r="N107" t="s">
         <v>30</v>
@@ -3730,7 +3730,7 @@
       </c>
       <c r="B108">
         <f t="shared" ca="1" si="3"/>
-        <v>0.98377146008644456</v>
+        <v>0.89312327633321698</v>
       </c>
       <c r="N108" t="s">
         <v>34</v>
@@ -3757,7 +3757,7 @@
       </c>
       <c r="B109">
         <f t="shared" ca="1" si="3"/>
-        <v>9.9946321624344581E-2</v>
+        <v>0.34695081386515247</v>
       </c>
       <c r="N109" t="s">
         <v>3</v>
@@ -3784,7 +3784,7 @@
       </c>
       <c r="B110">
         <f t="shared" ca="1" si="3"/>
-        <v>8.7545131137329424E-2</v>
+        <v>3.0171206547300988E-2</v>
       </c>
       <c r="N110" t="s">
         <v>14</v>
@@ -3811,7 +3811,7 @@
       </c>
       <c r="B111">
         <f t="shared" ca="1" si="3"/>
-        <v>0.64011423079773955</v>
+        <v>0.6975908758803987</v>
       </c>
       <c r="N111" t="s">
         <v>43</v>
@@ -3838,7 +3838,7 @@
       </c>
       <c r="B112">
         <f t="shared" ca="1" si="3"/>
-        <v>0.6561269508998282</v>
+        <v>0.20795035661962358</v>
       </c>
       <c r="N112" t="s">
         <v>42</v>
@@ -3865,7 +3865,7 @@
       </c>
       <c r="B113">
         <f t="shared" ca="1" si="3"/>
-        <v>0.81047186178569131</v>
+        <v>0.79922972114297097</v>
       </c>
       <c r="N113" t="s">
         <v>51</v>
@@ -3892,7 +3892,7 @@
       </c>
       <c r="B114">
         <f t="shared" ca="1" si="3"/>
-        <v>0.48581665741455227</v>
+        <v>0.73359592251234673</v>
       </c>
       <c r="N114" t="s">
         <v>20</v>
@@ -3919,7 +3919,7 @@
       </c>
       <c r="B115">
         <f t="shared" ca="1" si="3"/>
-        <v>0.31878541277308914</v>
+        <v>0.98710409212665728</v>
       </c>
       <c r="N115" t="s">
         <v>15</v>
@@ -3946,7 +3946,7 @@
       </c>
       <c r="B116">
         <f t="shared" ca="1" si="3"/>
-        <v>0.73258217538927384</v>
+        <v>0.75787822323670673</v>
       </c>
       <c r="N116" t="s">
         <v>16</v>
@@ -3973,7 +3973,7 @@
       </c>
       <c r="B117">
         <f t="shared" ca="1" si="3"/>
-        <v>0.14359544982951811</v>
+        <v>0.54423991105163927</v>
       </c>
       <c r="N117" t="s">
         <v>14</v>
@@ -4000,7 +4000,7 @@
       </c>
       <c r="B118">
         <f t="shared" ca="1" si="3"/>
-        <v>0.8628647760275393</v>
+        <v>0.84014225942207199</v>
       </c>
       <c r="N118" t="s">
         <v>45</v>
@@ -4027,7 +4027,7 @@
       </c>
       <c r="B119">
         <f t="shared" ca="1" si="3"/>
-        <v>0.96974554174346539</v>
+        <v>0.52025136893197876</v>
       </c>
       <c r="N119" t="s">
         <v>48</v>
@@ -4054,7 +4054,7 @@
       </c>
       <c r="B120">
         <f t="shared" ca="1" si="3"/>
-        <v>0.59130654959633744</v>
+        <v>0.34602356175598936</v>
       </c>
       <c r="N120" t="s">
         <v>38</v>
@@ -4081,7 +4081,7 @@
       </c>
       <c r="B121">
         <f t="shared" ca="1" si="3"/>
-        <v>9.7783300589130984E-2</v>
+        <v>0.66373730422176924</v>
       </c>
       <c r="N121" t="s">
         <v>36</v>
@@ -4108,7 +4108,7 @@
       </c>
       <c r="B122">
         <f t="shared" ca="1" si="3"/>
-        <v>0.33969904647028426</v>
+        <v>0.41005949309412182</v>
       </c>
       <c r="N122" t="s">
         <v>54</v>
@@ -4135,7 +4135,7 @@
       </c>
       <c r="B123">
         <f t="shared" ca="1" si="3"/>
-        <v>0.96113268375760408</v>
+        <v>0.10063902113995837</v>
       </c>
       <c r="N123" t="s">
         <v>10</v>
@@ -4162,7 +4162,7 @@
       </c>
       <c r="B124">
         <f t="shared" ca="1" si="3"/>
-        <v>0.26192779331566829</v>
+        <v>0.78515281357559674</v>
       </c>
       <c r="N124" t="s">
         <v>23</v>
@@ -4189,7 +4189,7 @@
       </c>
       <c r="B125">
         <f t="shared" ca="1" si="3"/>
-        <v>0.20685995771443677</v>
+        <v>0.82558883637365055</v>
       </c>
       <c r="N125" t="s">
         <v>21</v>
@@ -4216,7 +4216,7 @@
       </c>
       <c r="B126">
         <f t="shared" ca="1" si="3"/>
-        <v>3.2371408076637187E-2</v>
+        <v>0.35358833686086621</v>
       </c>
       <c r="N126" t="s">
         <v>8</v>
@@ -4243,7 +4243,7 @@
       </c>
       <c r="B127">
         <f t="shared" ca="1" si="3"/>
-        <v>0.31987464660502707</v>
+        <v>0.59175635021259287</v>
       </c>
       <c r="N127" t="s">
         <v>52</v>
@@ -4270,7 +4270,7 @@
       </c>
       <c r="B128">
         <f t="shared" ca="1" si="3"/>
-        <v>0.32024453262130304</v>
+        <v>0.83018985733652761</v>
       </c>
       <c r="N128" t="s">
         <v>1</v>
@@ -4297,7 +4297,7 @@
       </c>
       <c r="B129">
         <f t="shared" ref="B129:B160" ca="1" si="4">RAND()</f>
-        <v>0.83948595447265195</v>
+        <v>0.99312745859355311</v>
       </c>
       <c r="N129" t="s">
         <v>44</v>
@@ -4324,7 +4324,7 @@
       </c>
       <c r="B130">
         <f t="shared" ca="1" si="4"/>
-        <v>0.6486183432012369</v>
+        <v>0.3127023303797738</v>
       </c>
       <c r="N130" t="s">
         <v>52</v>
@@ -4351,7 +4351,7 @@
       </c>
       <c r="B131">
         <f t="shared" ca="1" si="4"/>
-        <v>0.26223900612742168</v>
+        <v>0.92936193367002673</v>
       </c>
       <c r="N131" t="s">
         <v>17</v>
@@ -4378,7 +4378,7 @@
       </c>
       <c r="B132">
         <f t="shared" ca="1" si="4"/>
-        <v>0.91451472544813972</v>
+        <v>0.24065444658544144</v>
       </c>
       <c r="N132" t="s">
         <v>53</v>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="B133">
         <f t="shared" ca="1" si="4"/>
-        <v>0.38432755429225762</v>
+        <v>0.61561256033212253</v>
       </c>
       <c r="N133" t="s">
         <v>55</v>
@@ -4432,7 +4432,7 @@
       </c>
       <c r="B134">
         <f t="shared" ca="1" si="4"/>
-        <v>0.48328609109848342</v>
+        <v>0.48892468712228498</v>
       </c>
       <c r="N134" t="s">
         <v>13</v>
@@ -4459,7 +4459,7 @@
       </c>
       <c r="B135">
         <f t="shared" ca="1" si="4"/>
-        <v>0.47352541472239607</v>
+        <v>0.45628811212074549</v>
       </c>
       <c r="N135" t="s">
         <v>3</v>
@@ -4486,7 +4486,7 @@
       </c>
       <c r="B136">
         <f t="shared" ca="1" si="4"/>
-        <v>0.32605611112536359</v>
+        <v>0.61713920772746733</v>
       </c>
       <c r="N136" t="s">
         <v>5</v>
@@ -4513,7 +4513,7 @@
       </c>
       <c r="B137">
         <f t="shared" ca="1" si="4"/>
-        <v>0.49256209413410279</v>
+        <v>0.24351799506295035</v>
       </c>
       <c r="N137" t="s">
         <v>25</v>
@@ -4540,7 +4540,7 @@
       </c>
       <c r="B138">
         <f t="shared" ca="1" si="4"/>
-        <v>0.60208581850005682</v>
+        <v>0.96742621056422917</v>
       </c>
       <c r="N138" t="s">
         <v>36</v>
@@ -4567,7 +4567,7 @@
       </c>
       <c r="B139">
         <f t="shared" ca="1" si="4"/>
-        <v>0.34324235641418055</v>
+        <v>6.04367265894451E-2</v>
       </c>
       <c r="N139" t="s">
         <v>34</v>
@@ -4594,7 +4594,7 @@
       </c>
       <c r="B140">
         <f t="shared" ca="1" si="4"/>
-        <v>0.32611993867402378</v>
+        <v>0.56393243685870242</v>
       </c>
       <c r="N140" t="s">
         <v>37</v>
@@ -4621,7 +4621,7 @@
       </c>
       <c r="B141">
         <f t="shared" ca="1" si="4"/>
-        <v>0.52710030886461046</v>
+        <v>0.20623288364193471</v>
       </c>
       <c r="N141" t="s">
         <v>24</v>
@@ -4648,7 +4648,7 @@
       </c>
       <c r="B142">
         <f t="shared" ca="1" si="4"/>
-        <v>0.32529824528052353</v>
+        <v>0.9293248025022659</v>
       </c>
       <c r="N142" t="s">
         <v>35</v>
@@ -4675,7 +4675,7 @@
       </c>
       <c r="B143">
         <f t="shared" ca="1" si="4"/>
-        <v>0.54861178813098732</v>
+        <v>0.58983367046693969</v>
       </c>
       <c r="N143" t="s">
         <v>8</v>
@@ -4702,7 +4702,7 @@
       </c>
       <c r="B144">
         <f t="shared" ca="1" si="4"/>
-        <v>0.11661412047657782</v>
+        <v>0.10880267888907114</v>
       </c>
       <c r="N144" t="s">
         <v>28</v>
@@ -4729,7 +4729,7 @@
       </c>
       <c r="B145">
         <f t="shared" ca="1" si="4"/>
-        <v>0.99113906052094136</v>
+        <v>0.54709681527835619</v>
       </c>
       <c r="N145" t="s">
         <v>35</v>
@@ -4756,7 +4756,7 @@
       </c>
       <c r="B146">
         <f t="shared" ca="1" si="4"/>
-        <v>9.4251221601392432E-2</v>
+        <v>0.32745164871925625</v>
       </c>
       <c r="N146" t="s">
         <v>0</v>
@@ -4783,7 +4783,7 @@
       </c>
       <c r="B147">
         <f t="shared" ca="1" si="4"/>
-        <v>0.57329964708244652</v>
+        <v>0.63318124835994594</v>
       </c>
       <c r="N147" t="s">
         <v>27</v>
@@ -4810,7 +4810,7 @@
       </c>
       <c r="B148">
         <f t="shared" ca="1" si="4"/>
-        <v>0.53946108889684197</v>
+        <v>0.28576143209366323</v>
       </c>
       <c r="N148" t="s">
         <v>9</v>
@@ -4837,7 +4837,7 @@
       </c>
       <c r="B149">
         <f t="shared" ca="1" si="4"/>
-        <v>2.0506662837521894E-2</v>
+        <v>0.66483889339214031</v>
       </c>
       <c r="N149" t="s">
         <v>11</v>
@@ -4864,7 +4864,7 @@
       </c>
       <c r="B150">
         <f t="shared" ca="1" si="4"/>
-        <v>0.63989136662043189</v>
+        <v>0.41192907935671552</v>
       </c>
       <c r="N150" t="s">
         <v>22</v>
@@ -4891,7 +4891,7 @@
       </c>
       <c r="B151">
         <f t="shared" ca="1" si="4"/>
-        <v>0.54538965928541816</v>
+        <v>0.76545788626430933</v>
       </c>
       <c r="N151" t="s">
         <v>30</v>
@@ -4918,7 +4918,7 @@
       </c>
       <c r="B152">
         <f t="shared" ca="1" si="4"/>
-        <v>0.59009728040269693</v>
+        <v>0.1660587653076514</v>
       </c>
       <c r="N152" t="s">
         <v>56</v>
@@ -4945,7 +4945,7 @@
       </c>
       <c r="B153">
         <f t="shared" ca="1" si="4"/>
-        <v>0.24300892164472965</v>
+        <v>0.39369545198750866</v>
       </c>
       <c r="N153" t="s">
         <v>7</v>
@@ -4972,7 +4972,7 @@
       </c>
       <c r="B154">
         <f t="shared" ca="1" si="4"/>
-        <v>0.57967826329910976</v>
+        <v>0.40197289945723436</v>
       </c>
       <c r="N154" t="s">
         <v>12</v>
@@ -4999,7 +4999,7 @@
       </c>
       <c r="B155">
         <f t="shared" ca="1" si="4"/>
-        <v>0.48584016457206403</v>
+        <v>0.72851635574651508</v>
       </c>
       <c r="N155" t="s">
         <v>50</v>
@@ -5026,7 +5026,7 @@
       </c>
       <c r="B156">
         <f t="shared" ca="1" si="4"/>
-        <v>0.59662498616055737</v>
+        <v>0.49931185812103029</v>
       </c>
       <c r="N156" t="s">
         <v>42</v>
@@ -5053,7 +5053,7 @@
       </c>
       <c r="B157">
         <f t="shared" ca="1" si="4"/>
-        <v>0.60898228663912035</v>
+        <v>0.53214590489564217</v>
       </c>
       <c r="N157" t="s">
         <v>44</v>
@@ -5080,7 +5080,7 @@
       </c>
       <c r="B158">
         <f t="shared" ca="1" si="4"/>
-        <v>0.49637536354523937</v>
+        <v>0.76461826499189856</v>
       </c>
       <c r="N158" t="s">
         <v>56</v>
@@ -5107,7 +5107,7 @@
       </c>
       <c r="B159">
         <f t="shared" ca="1" si="4"/>
-        <v>0.27562294506825324</v>
+        <v>0.52939193743217372</v>
       </c>
       <c r="N159" t="s">
         <v>29</v>
@@ -5134,7 +5134,7 @@
       </c>
       <c r="B160">
         <f t="shared" ca="1" si="4"/>
-        <v>0.8601688576913914</v>
+        <v>0.80774298439239944</v>
       </c>
       <c r="N160" t="s">
         <v>51</v>
@@ -5161,7 +5161,7 @@
       </c>
       <c r="B161">
         <f t="shared" ref="B161:B171" ca="1" si="5">RAND()</f>
-        <v>0.14056254765138776</v>
+        <v>0.60158465542077832</v>
       </c>
       <c r="N161" t="s">
         <v>32</v>
@@ -5188,7 +5188,7 @@
       </c>
       <c r="B162">
         <f t="shared" ca="1" si="5"/>
-        <v>0.84321984220121926</v>
+        <v>0.81172108248775798</v>
       </c>
       <c r="N162" t="s">
         <v>21</v>
@@ -5215,7 +5215,7 @@
       </c>
       <c r="B163">
         <f t="shared" ca="1" si="5"/>
-        <v>0.63246193441893894</v>
+        <v>8.8516546351903647E-2</v>
       </c>
       <c r="N163" t="s">
         <v>42</v>
@@ -5242,7 +5242,7 @@
       </c>
       <c r="B164">
         <f t="shared" ca="1" si="5"/>
-        <v>0.16533510248882333</v>
+        <v>0.63888223473540373</v>
       </c>
       <c r="N164" t="s">
         <v>26</v>
@@ -5269,7 +5269,7 @@
       </c>
       <c r="B165">
         <f t="shared" ca="1" si="5"/>
-        <v>0.35746736133557067</v>
+        <v>0.42359848174661108</v>
       </c>
       <c r="N165" t="s">
         <v>45</v>
@@ -5296,7 +5296,7 @@
       </c>
       <c r="B166">
         <f t="shared" ca="1" si="5"/>
-        <v>0.50279055484406809</v>
+        <v>0.60452497019098606</v>
       </c>
       <c r="N166" t="s">
         <v>10</v>
@@ -5323,7 +5323,7 @@
       </c>
       <c r="B167">
         <f t="shared" ca="1" si="5"/>
-        <v>0.734812849340858</v>
+        <v>0.95560286561357699</v>
       </c>
       <c r="N167" t="s">
         <v>37</v>
@@ -5350,7 +5350,7 @@
       </c>
       <c r="B168">
         <f t="shared" ca="1" si="5"/>
-        <v>0.64219526038976038</v>
+        <v>0.5655562557108621</v>
       </c>
       <c r="N168" t="s">
         <v>48</v>
@@ -5377,7 +5377,7 @@
       </c>
       <c r="B169">
         <f t="shared" ca="1" si="5"/>
-        <v>0.40777499444212806</v>
+        <v>0.74760489001514208</v>
       </c>
       <c r="N169" t="s">
         <v>26</v>
@@ -5404,7 +5404,7 @@
       </c>
       <c r="B170">
         <f t="shared" ca="1" si="5"/>
-        <v>8.328043353181469E-2</v>
+        <v>0.56330091044017261</v>
       </c>
       <c r="N170" t="s">
         <v>30</v>
@@ -5431,7 +5431,7 @@
       </c>
       <c r="B171">
         <f t="shared" ca="1" si="5"/>
-        <v>0.43130709536089817</v>
+        <v>0.79876945490575268</v>
       </c>
       <c r="N171" t="s">
         <v>12</v>
@@ -5476,7 +5476,7 @@
       </c>
       <c r="B1">
         <f t="shared" ref="B1:B21" ca="1" si="0">RAND()</f>
-        <v>4.45986430113543E-3</v>
+        <v>0.86055744499821651</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -5485,7 +5485,7 @@
       </c>
       <c r="B2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.98559854458366092</v>
+        <v>0.45528057088116336</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -5494,7 +5494,7 @@
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="0"/>
-        <v>4.1661003511263783E-2</v>
+        <v>5.3395837375365796E-2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -5503,7 +5503,7 @@
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.7586589981955344</v>
+        <v>0.46141005053364637</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -5512,7 +5512,7 @@
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.97843846208428742</v>
+        <v>0.40545743453028882</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -5521,7 +5521,7 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.1043274946057704</v>
+        <v>0.1553724720369567</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -5530,7 +5530,7 @@
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.16794181205985237</v>
+        <v>0.88477108286615369</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -5539,7 +5539,7 @@
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.23458817096178386</v>
+        <v>0.42387694855251778</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -5548,7 +5548,7 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>0.93551980931408285</v>
+        <v>0.88753319830629229</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -5557,7 +5557,7 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>0.91842750230380543</v>
+        <v>3.305139483454389E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -5566,7 +5566,7 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.5940314042043644</v>
+        <v>0.89056346294263034</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -5575,7 +5575,7 @@
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.37311024131744508</v>
+        <v>0.96451060093472096</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -5584,7 +5584,7 @@
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.9112915965772187</v>
+        <v>0.97518978816105406</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -5593,7 +5593,7 @@
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>0.31971004268080194</v>
+        <v>0.69567494463523538</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -5602,7 +5602,7 @@
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>0.63366007266950286</v>
+        <v>0.59816972745958019</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -5611,7 +5611,7 @@
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.86181123674044513</v>
+        <v>0.73536194894551909</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -5620,7 +5620,7 @@
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="0"/>
-        <v>0.31679852153587484</v>
+        <v>0.96646388858284682</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -5629,7 +5629,7 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="0"/>
-        <v>0.22899202682718234</v>
+        <v>0.77280681035482002</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -5638,7 +5638,7 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="0"/>
-        <v>0.31159764422781966</v>
+        <v>0.79917976088973175</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -5647,7 +5647,7 @@
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="0"/>
-        <v>0.78049205571326552</v>
+        <v>0.12286215605690876</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -5656,7 +5656,7 @@
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="0"/>
-        <v>0.45705497951220342</v>
+        <v>0.23527803473909947</v>
       </c>
     </row>
   </sheetData>
@@ -5671,7 +5671,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{060B1769-110F-44D1-9F20-919BEAF24A80}">
   <dimension ref="A1:C3107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="Q1" zoomScale="45" zoomScaleNormal="45" workbookViewId="0">
       <selection activeCell="C17" sqref="C17:C646"/>
     </sheetView>
   </sheetViews>

</xml_diff>